<commit_message>
I have added a coulum as Day_brood interval for all exposures
</commit_message>
<xml_diff>
--- a/Tai/Tia_Metadata.xlsx
+++ b/Tai/Tia_Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b3bbfbef5e37dc7/Documents/R_PHD_analysis/Multigenerational_analysis/life-history-traits-analysis/Tai/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\200240958\Desktop\GitHubProjects\ChronicExposure\Tai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B073224-A085-4FF7-BBF8-B6EEAFE4FAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAA27D8-7F5A-4C0C-9989-2F980D1AB739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{52BA6A10-123A-43EE-869B-F79B31AC3FB5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{52BA6A10-123A-43EE-869B-F79B31AC3FB5}"/>
   </bookViews>
   <sheets>
     <sheet name="MP" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="28">
   <si>
     <t>ReplicatesGenotypesTreatmentAge of maturation</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Day_brood interval</t>
+  </si>
+  <si>
+    <t>Day_interval</t>
+  </si>
+  <si>
+    <t>Day_ brood interval</t>
   </si>
 </sst>
 </file>
@@ -471,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42034C1-5798-4672-8953-A9046EE04A5F}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,8 +513,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -537,8 +549,11 @@
         <f>(F2+I2)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -567,11 +582,14 @@
         <v>20</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J17" si="0">(F3+I3)</f>
+        <f t="shared" ref="J3:J5" si="0">(F3+I3)</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -603,8 +621,11 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -636,8 +657,11 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -669,8 +693,11 @@
         <f>(F6+I6)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -702,8 +729,11 @@
         <f>(F7+I7)</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -735,8 +765,11 @@
         <f>(F8+I8)</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -768,8 +801,11 @@
         <f>(F9+I9)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -801,8 +837,11 @@
         <f>(F10+I10)</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -816,7 +855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -848,8 +887,11 @@
         <f>(F12+I12)</f>
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
@@ -881,8 +923,11 @@
         <f>(F13+I13)</f>
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -909,7 +954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -920,7 +965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -952,8 +997,11 @@
         <f>(F16+I16)</f>
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -984,6 +1032,9 @@
       <c r="J17">
         <f>(F17+I17)</f>
         <v>23</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -993,15 +1044,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9884E5-3085-460D-964B-080D59FFBE10}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K1" sqref="K1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1026,8 +1077,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1059,8 +1113,11 @@
         <f>(F2+I2)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1092,8 +1149,11 @@
         <f>(F3+I3)</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1122,11 +1182,14 @@
         <v>26</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J17" si="0">(F4+I4)</f>
+        <f t="shared" ref="J4:J5" si="0">(F4+I4)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1158,8 +1221,11 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1188,11 +1254,14 @@
         <v>19</v>
       </c>
       <c r="J6">
-        <f>(F6+I6)</f>
+        <f t="shared" ref="J6:J17" si="1">(F6+I6)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1221,11 +1290,14 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <f>(F7+I7)</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1254,11 +1326,14 @@
         <v>22</v>
       </c>
       <c r="J8">
-        <f>(F8+I8)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1287,11 +1362,14 @@
         <v>28</v>
       </c>
       <c r="J9">
-        <f>(F9+I9)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1320,11 +1398,14 @@
         <v>14</v>
       </c>
       <c r="J10">
-        <f>(F10+I10)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1353,11 +1434,14 @@
         <v>17</v>
       </c>
       <c r="J11">
-        <f>(F11+I11)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1386,11 +1470,14 @@
         <v>22</v>
       </c>
       <c r="J12">
-        <f>(F12+I12)</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1419,11 +1506,14 @@
         <v>6</v>
       </c>
       <c r="J13">
-        <f>(F13+I13)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1452,11 +1542,14 @@
         <v>17</v>
       </c>
       <c r="J14">
-        <f>(F14+I14)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1485,11 +1578,14 @@
         <v>1</v>
       </c>
       <c r="J15">
-        <f>(F15+I15)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1518,11 +1614,14 @@
         <v>21</v>
       </c>
       <c r="J16">
-        <f>(F16+I16)</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1551,8 +1650,11 @@
         <v>11</v>
       </c>
       <c r="J17">
-        <f>(F17+I17)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
+      </c>
+      <c r="K17">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1562,15 +1664,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C28442-DD13-40D7-AA91-81015BD29E98}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="K1" sqref="K1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1595,8 +1697,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1628,8 +1733,11 @@
         <f>(F2+I2)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1658,11 +1766,14 @@
         <v>20</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J17" si="0">(F3+I3)</f>
+        <f t="shared" ref="J3:J5" si="0">(F3+I3)</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1694,8 +1805,11 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1727,8 +1841,11 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1760,8 +1877,11 @@
         <f>(F6+I6)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1793,8 +1913,11 @@
         <f>(F7+I7)</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1826,8 +1949,11 @@
         <f>(F8+I8)</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1859,8 +1985,11 @@
         <f>(F9+I9)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1887,7 +2016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1901,7 +2030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1933,8 +2062,11 @@
         <f>(F12+I12)</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1966,8 +2098,11 @@
         <f>(F13+I13)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1999,8 +2134,11 @@
         <f>(F14+I14)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2011,7 +2149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2043,8 +2181,11 @@
         <f>(F16+I16)</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2075,6 +2216,9 @@
       <c r="J17">
         <f>(F17+I17)</f>
         <v>28</v>
+      </c>
+      <c r="K17">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2084,15 +2228,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EBCCFF-0435-42C6-BDFA-FB0BCE3A96B4}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="K1" sqref="K1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2117,8 +2261,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2150,8 +2297,11 @@
         <f>(F2+I2)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2183,8 +2333,11 @@
         <f t="shared" ref="J3:J17" si="0">(F3+I3)</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2216,8 +2369,11 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2249,8 +2405,11 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2279,11 +2438,14 @@
         <v>19</v>
       </c>
       <c r="J6">
-        <f>(F6+I6)</f>
+        <f t="shared" ref="J6:J12" si="1">(F6+I6)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2312,11 +2474,14 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <f>(F7+I7)</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2345,11 +2510,14 @@
         <v>22</v>
       </c>
       <c r="J8">
-        <f>(F8+I8)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2378,11 +2546,14 @@
         <v>28</v>
       </c>
       <c r="J9">
-        <f>(F9+I9)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2411,11 +2582,14 @@
         <v>19</v>
       </c>
       <c r="J10">
-        <f>(F10+I10)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2444,11 +2618,14 @@
         <v>20</v>
       </c>
       <c r="J11">
-        <f>(F11+I11)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -2477,11 +2654,14 @@
         <v>10</v>
       </c>
       <c r="J12">
-        <f>(F12+I12)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
@@ -2492,7 +2672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2524,8 +2704,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2557,8 +2740,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2590,8 +2776,11 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2622,6 +2811,9 @@
       <c r="J17">
         <f t="shared" si="0"/>
         <v>17</v>
+      </c>
+      <c r="K17">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2631,15 +2823,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F5938C-5964-47CC-92DA-F67B5FC064A9}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K1" sqref="K1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2664,8 +2856,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2697,8 +2892,11 @@
         <f>(F2+I2)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2727,11 +2925,14 @@
         <v>20</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J17" si="0">(F3+I3)</f>
+        <f t="shared" ref="J3:J5" si="0">(F3+I3)</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2763,8 +2964,11 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2796,8 +3000,11 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2829,8 +3036,11 @@
         <f>(F6+I6)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2862,8 +3072,11 @@
         <f>(F7+I7)</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2895,8 +3108,11 @@
         <f>(F8+I8)</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2928,8 +3144,11 @@
         <f>(F9+I9)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2961,8 +3180,11 @@
         <f>(F10+I10)</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2976,7 +3198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -3005,11 +3227,14 @@
         <v>9</v>
       </c>
       <c r="J12">
-        <f>(F12+I12)</f>
+        <f t="shared" ref="J12:J17" si="1">(F12+I12)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
@@ -3038,11 +3263,14 @@
         <v>17</v>
       </c>
       <c r="J13">
-        <f>(F13+I13)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3071,11 +3299,14 @@
         <v>9</v>
       </c>
       <c r="J14">
-        <f>(F14+I14)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3104,11 +3335,14 @@
         <v>8</v>
       </c>
       <c r="J15">
-        <f>(F15+I15)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3137,11 +3371,14 @@
         <v>10</v>
       </c>
       <c r="J16">
-        <f>(F16+I16)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -3170,8 +3407,11 @@
         <v>8</v>
       </c>
       <c r="J17">
-        <f>(F17+I17)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3181,15 +3421,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EC2BFA-F622-41CC-81FC-AF536E230620}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K1" sqref="K1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3214,8 +3454,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3247,8 +3490,11 @@
         <f>(F2+I2)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3277,11 +3523,14 @@
         <v>20</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J17" si="0">(F3+I3)</f>
+        <f t="shared" ref="J3:J5" si="0">(F3+I3)</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3313,8 +3562,11 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3346,8 +3598,11 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3376,11 +3631,14 @@
         <v>19</v>
       </c>
       <c r="J6">
-        <f>(F6+I6)</f>
+        <f t="shared" ref="J6:J17" si="1">(F6+I6)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -3409,11 +3667,14 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <f>(F7+I7)</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -3442,11 +3703,14 @@
         <v>22</v>
       </c>
       <c r="J8">
-        <f>(F8+I8)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -3475,11 +3739,14 @@
         <v>28</v>
       </c>
       <c r="J9">
-        <f>(F9+I9)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3508,11 +3775,14 @@
         <v>16</v>
       </c>
       <c r="J10">
-        <f>(F10+I10)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3541,11 +3811,14 @@
         <v>9</v>
       </c>
       <c r="J11">
-        <f>(F11+I11)</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -3574,11 +3847,14 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <f>(F12+I12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
@@ -3607,11 +3883,14 @@
         <v>11</v>
       </c>
       <c r="J13">
-        <f>(F13+I13)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3640,11 +3919,14 @@
         <v>10</v>
       </c>
       <c r="J14">
-        <f>(F14+I14)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3673,11 +3955,14 @@
         <v>5</v>
       </c>
       <c r="J15">
-        <f>(F15+I15)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3706,11 +3991,14 @@
         <v>6</v>
       </c>
       <c r="J16">
-        <f>(F16+I16)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -3739,8 +4027,11 @@
         <v>4</v>
       </c>
       <c r="J17">
-        <f>(F17+I17)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
+      </c>
+      <c r="K17">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3750,15 +4041,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA5DD5B-DA17-4C47-9DB1-1A2DE71E5699}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3783,8 +4074,11 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3816,8 +4110,11 @@
         <f>(F2+I2)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3849,8 +4146,11 @@
         <f t="shared" ref="J3:J16" si="0">(F3+I3)</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3882,8 +4182,11 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3915,8 +4218,11 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3945,11 +4251,14 @@
         <v>19</v>
       </c>
       <c r="J6">
-        <f>(F6+I6)</f>
+        <f t="shared" ref="J6:J13" si="1">(F6+I6)</f>
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -3978,11 +4287,14 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <f>(F7+I7)</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -4011,11 +4323,14 @@
         <v>22</v>
       </c>
       <c r="J8">
-        <f>(F8+I8)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -4044,11 +4359,14 @@
         <v>28</v>
       </c>
       <c r="J9">
-        <f>(F9+I9)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4077,11 +4395,14 @@
         <v>17</v>
       </c>
       <c r="J10">
-        <f>(F10+I10)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -4110,11 +4431,14 @@
         <v>18</v>
       </c>
       <c r="J11">
-        <f>(F11+I11)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -4143,11 +4467,14 @@
         <v>4</v>
       </c>
       <c r="J12">
-        <f>(F12+I12)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
@@ -4176,11 +4503,14 @@
         <v>10</v>
       </c>
       <c r="J13">
-        <f>(F13+I13)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -4198,7 +4528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -4216,7 +4546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -4237,7 +4567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -4267,6 +4597,9 @@
       </c>
       <c r="J17">
         <v>4</v>
+      </c>
+      <c r="K17">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>